<commit_message>
Remove duplicate 'vegetable oil'
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="71">
   <si>
     <t xml:space="preserve">f_crop</t>
   </si>
@@ -214,28 +214,28 @@
     <t xml:space="preserve">potatoe protein</t>
   </si>
   <si>
+    <t xml:space="preserve">fish meal</t>
+  </si>
+  <si>
     <t xml:space="preserve">linseed</t>
   </si>
   <si>
+    <t xml:space="preserve">luzern meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">palm kernel expeller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soybean meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soybean protein concentrate</t>
+  </si>
+  <si>
     <t xml:space="preserve">soybeans</t>
   </si>
   <si>
-    <t xml:space="preserve">soybean meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soybean protein concentrate</t>
-  </si>
-  <si>
     <t xml:space="preserve">sunflower seed meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">palm kernel expeller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">luzern meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fish meal</t>
   </si>
 </sst>
 </file>
@@ -366,6 +366,23 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -4587,10 +4604,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5069,7 +5086,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>33</v>
@@ -5083,7 +5100,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>33</v>
@@ -5097,7 +5114,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>33</v>
@@ -5111,7 +5128,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>33</v>
@@ -5125,7 +5142,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>33</v>
@@ -5139,7 +5156,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>33</v>
@@ -5153,7 +5170,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>33</v>
@@ -5166,26 +5183,8 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0"/>
-      <c r="B44" s="0"/>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0"/>
-      <c r="B45" s="0"/>
+      <c r="A43" s="0"/>
+      <c r="B43" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="1"/>
@@ -5230,10 +5229,6 @@
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0"/>
-      <c r="B57" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Update FeedMgmt, drop whey
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -12,6 +12,7 @@
     <sheet name="DemandAndConversions" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="CropProduction" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="CattleHerd" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="FeedMgmt" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="80">
   <si>
     <t xml:space="preserve">f_crop</t>
   </si>
@@ -184,27 +185,51 @@
     <t xml:space="preserve">wheat bran, fine</t>
   </si>
   <si>
+    <t xml:space="preserve">fish meal</t>
+  </si>
+  <si>
     <t xml:space="preserve">oat hulls</t>
   </si>
   <si>
+    <t xml:space="preserve">linseed</t>
+  </si>
+  <si>
     <t xml:space="preserve">oat bran</t>
   </si>
   <si>
+    <t xml:space="preserve">luzern meal</t>
+  </si>
+  <si>
     <t xml:space="preserve">rye bran</t>
   </si>
   <si>
+    <t xml:space="preserve">palm kernel expeller</t>
+  </si>
+  <si>
     <t xml:space="preserve">wheat distillers grain, dry</t>
   </si>
   <si>
+    <t xml:space="preserve">soybean meal</t>
+  </si>
+  <si>
     <t xml:space="preserve">barley brewers grain</t>
   </si>
   <si>
+    <t xml:space="preserve">soybean protein concentrate</t>
+  </si>
+  <si>
     <t xml:space="preserve">maize gluten meal</t>
   </si>
   <si>
+    <t xml:space="preserve">soybeans</t>
+  </si>
+  <si>
     <t xml:space="preserve">sugar beet molasses</t>
   </si>
   <si>
+    <t xml:space="preserve">sunflower seed meal</t>
+  </si>
+  <si>
     <t xml:space="preserve">sugar beet pulp</t>
   </si>
   <si>
@@ -214,28 +239,31 @@
     <t xml:space="preserve">potatoe protein</t>
   </si>
   <si>
-    <t xml:space="preserve">fish meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">linseed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">luzern meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">palm kernel expeller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soybean meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soybean protein concentrate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soybeans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sunflower seed meal</t>
+    <t xml:space="preserve">f_species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f_crop_prod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f_by_prod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cattle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">share_domestic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">milling by-products from wheat, barley or rye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wheat distillers grain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">whey</t>
   </si>
 </sst>
 </file>
@@ -366,23 +394,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -565,7 +576,7 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -644,8 +655,8 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -749,8 +760,8 @@
   </sheetPr>
   <dimension ref="A1:G231"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4604,10 +4615,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4923,10 +4934,22 @@
       <c r="D23" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="H23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>33</v>
@@ -4937,10 +4960,22 @@
       <c r="D24" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="H24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>33</v>
@@ -4951,10 +4986,22 @@
       <c r="D25" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="H25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>33</v>
@@ -4965,10 +5012,22 @@
       <c r="D26" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="H26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K26" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>33</v>
@@ -4979,10 +5038,22 @@
       <c r="D27" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="H27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>33</v>
@@ -4993,10 +5064,22 @@
       <c r="D28" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="H28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K28" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>33</v>
@@ -5007,10 +5090,22 @@
       <c r="D29" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="H29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K29" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>33</v>
@@ -5021,10 +5116,22 @@
       <c r="D30" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="H30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K30" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>33</v>
@@ -5038,7 +5145,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>33</v>
@@ -5052,7 +5159,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>33</v>
@@ -5069,122 +5176,6 @@
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0"/>
-      <c r="B43" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="1"/>
@@ -5239,4 +5230,524 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q27"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="14.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="42.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="8.59"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="K19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M19" s="1"/>
+      <c r="N19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q19" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="K20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M20" s="1"/>
+      <c r="N20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q20" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q22" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="3"/>
+      <c r="K23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q23" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="3"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update scenario files - base scenario works now
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="85">
   <si>
     <t xml:space="preserve">f_crop</t>
   </si>
@@ -158,112 +158,127 @@
     <t xml:space="preserve">rye</t>
   </si>
   <si>
+    <t xml:space="preserve">peas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">broad beans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rapeseed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vegetable oils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rapeseed meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rapeseed cake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wheat bran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wheat bran, fine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oat hulls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oat bran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rye bran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wheat distillers grain, dry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barley brewers grain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maize gluten meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sugar beet molasses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sugar beet pulp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">potatoe protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">luzern meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sunflower seed meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">palm kern expeller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wheat distillers grain, wet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">whey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fish meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soybean protein concentrated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">whey powder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f_species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f_crop_prod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f_by_prod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cattle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soybeans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">share_domestic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linseed</t>
+  </si>
+  <si>
     <t xml:space="preserve">maize</t>
   </si>
   <si>
-    <t xml:space="preserve">peas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">broad beans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rapeseed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vegetable oils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rapeseed meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rapeseed cake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wheat bran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wheat bran, fine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fish meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oat hulls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">linseed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oat bran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">luzern meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rye bran</t>
+    <t xml:space="preserve">milling by-products from wheat, barley or rye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soybean meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soybean protein concentrate</t>
   </si>
   <si>
     <t xml:space="preserve">palm kernel expeller</t>
   </si>
   <si>
-    <t xml:space="preserve">wheat distillers grain, dry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soybean meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">barley brewers grain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soybean protein concentrate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maize gluten meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soybeans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sugar beet molasses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sunflower seed meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sugar beet pulp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">whey powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">potatoe protein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f_species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f_crop_prod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f_by_prod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cattle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">share_domestic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">milling by-products from wheat, barley or rye</t>
-  </si>
-  <si>
     <t xml:space="preserve">organic</t>
   </si>
   <si>
     <t xml:space="preserve">wheat distillers grain</t>
   </si>
   <si>
-    <t xml:space="preserve">whey</t>
+    <t xml:space="preserve">milling by-products from oats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">potatoe offals</t>
   </si>
 </sst>
 </file>
@@ -360,7 +375,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -377,12 +392,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -576,7 +595,7 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -655,14 +674,14 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -760,8 +779,8 @@
   </sheetPr>
   <dimension ref="A1:G231"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A75" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4615,15 +4634,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4656,570 +4677,527 @@
       <c r="D3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4" t="n">
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="4" t="n">
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="4" t="n">
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="4" t="n">
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="4" t="n">
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="4" t="n">
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="4" t="n">
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="4" t="n">
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="4" t="n">
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="4" t="n">
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="4" t="n">
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="4" t="n">
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="4" t="n">
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="4" t="n">
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="4" t="n">
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="4" t="n">
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="4" t="n">
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="4" t="n">
+      <c r="C21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="4" t="n">
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="4" t="n">
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K23" s="1" t="n">
+      <c r="C24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="1" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+      <c r="E24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="4" t="n">
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K24" s="1" t="n">
+      <c r="C26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="1" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
+      <c r="E26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="4" t="n">
+      <c r="C27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K25" s="1" t="n">
+      <c r="C28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="1" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="4" t="n">
+      <c r="C29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K26" s="1" t="n">
+      <c r="C30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="1" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
+      <c r="E30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="4" t="n">
+      <c r="C31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="G32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K27" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="1" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K28" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="1" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G36" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K29" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" s="1" t="s">
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G38" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K30" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G39" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5237,33 +5215,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="14.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="42.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="44.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -5275,64 +5252,64 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="3" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="3" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="3" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -5341,7 +5318,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -5350,404 +5327,353 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G9" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G11" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G12" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G14" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="3" t="n">
+      <c r="F15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G17" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G19" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="K19" s="1" t="s">
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M19" s="1"/>
-      <c r="N19" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="O19" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="P19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q19" s="3" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G20" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="K20" s="1" t="s">
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M20" s="1"/>
-      <c r="N20" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="P20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q20" s="3" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G21" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="H21" s="4"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K22" s="1" t="s">
+      <c r="H21" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="L22" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O22" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="P22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q22" s="3" t="n">
+      <c r="F23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="1" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="3"/>
-      <c r="K23" s="1" t="s">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L23" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="O23" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="P23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q23" s="3" t="n">
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="1" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="3"/>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>